<commit_message>
TD-937 Fix test data file replacing registrations with enrolments
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Web.Tests/TestData/ActivityDataDownloadTest.xlsx
+++ b/DigitalLearningSolutions.Web.Tests/TestData/ActivityDataDownloadTest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HEE\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\digitallearningsolutions\DigitalLearningSolutions.Web.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC2F99-3B83-4C20-902D-BBF6852C2B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8232"/>
+    <workbookView xWindow="-28898" yWindow="6278" windowWidth="28996" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usage Statistics" sheetId="2" r:id="rId1"/>
@@ -24,9 +25,6 @@
     <t>Period</t>
   </si>
   <si>
-    <t>Registrations</t>
-  </si>
-  <si>
     <t>Completions</t>
   </si>
   <si>
@@ -70,12 +68,15 @@
   </si>
   <si>
     <t>01/08/2021</t>
+  </si>
+  <si>
+    <t>Enrolments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,8 +106,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,13 +130,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0">
-  <autoFilter ref="A1:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0">
+  <autoFilter ref="A1:D14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Period" dataDxfId="0"/>
-    <tableColumn id="2" name="Registrations"/>
-    <tableColumn id="3" name="Completions"/>
-    <tableColumn id="4" name="Evaluations"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Period" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enrolments"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completions"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Evaluations"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -425,39 +426,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1015625" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" customWidth="1"/>
-    <col min="3" max="3" width="15.26171875" customWidth="1"/>
-    <col min="4" max="4" width="14.3125" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B2">
         <v>0</v>
       </c>
@@ -468,37 +469,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -510,108 +511,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
       <c r="B13">
         <v>0</v>
       </c>
@@ -622,9 +623,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>0</v>

</xml_diff>

<commit_message>
TD-4469 Limits details query by learner centre ID and updates related tests
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Web.Tests/TestData/ActivityDataDownloadTest.xlsx
+++ b/DigitalLearningSolutions.Web.Tests/TestData/ActivityDataDownloadTest.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\digitallearningsolutions\DigitalLearningSolutions.Web.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\DLSV2\DigitalLearningSolutions.Web.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC2F99-3B83-4C20-902D-BBF6852C2B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6958A-228B-4BA5-9C1B-494A48996351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="6278" windowWidth="28996" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Usage Statistics" sheetId="2" r:id="rId1"/>
+    <sheet name="Usage summary" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>